<commit_message>
Fixed calculation in template
</commit_message>
<xml_diff>
--- a/StuR-Generator/Data/Template.xlsx
+++ b/StuR-Generator/Data/Template.xlsx
@@ -5708,7 +5708,7 @@
   <dimension ref="A1:S41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M42" sqref="M42"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7050,7 +7050,7 @@
       </c>
       <c r="P25" s="14">
         <f>Q30</f>
-        <v>0</v>
+        <v>-1900</v>
       </c>
       <c r="Q25" s="15">
         <f>IF(N35=0,O25,IF(N35=A34,P25,O25-((O25-P25)/N35)*(A34)))</f>
@@ -7327,9 +7327,17 @@
         <f>IF(ISBLANK(Eingabe!M30), "",(480+Eingabe!M30)/60)</f>
         <v/>
       </c>
+      <c r="O30">
+        <f>A34</f>
+        <v>-25</v>
+      </c>
+      <c r="P30">
+        <f>O30-N35</f>
+        <v>-25</v>
+      </c>
       <c r="Q30" s="18">
         <f>(8-O35)*P30</f>
-        <v>0</v>
+        <v>-1900</v>
       </c>
       <c r="R30" s="19">
         <f>(A35-O35)*P30</f>
@@ -7390,7 +7398,7 @@
       </c>
       <c r="Q31" s="18">
         <f>Q30*60</f>
-        <v>0</v>
+        <v>-114000</v>
       </c>
       <c r="R31" s="19">
         <f>R30*60</f>
@@ -7457,7 +7465,7 @@
       </c>
       <c r="Q32" s="20">
         <f>Q30/8</f>
-        <v>0</v>
+        <v>-237.5</v>
       </c>
       <c r="R32" s="21">
         <f>R30/8</f>
@@ -7653,7 +7661,7 @@
       </c>
       <c r="O35">
         <f>IF(O30=N35,O33,O33/(O30-N35))</f>
-        <v>1700</v>
+        <v>-68</v>
       </c>
       <c r="Q35">
         <v>0</v>

</xml_diff>